<commit_message>
- Fixed a regex issue - Updated project metadata and argument names
</commit_message>
<xml_diff>
--- a/Test/Validation_Testdata.xlsx
+++ b/Test/Validation_Testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fan.zhang\Documents\preBuild\PopulateWordTemplatesWithCSV\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F2AC75-95BA-4E90-9D8A-A8073B41FF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD09202-312F-465F-B617-AC48B5FF589A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8415" yWindow="5610" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>